<commit_message>
update for new biosteam
</commit_message>
<xml_diff>
--- a/exposan/bwaise/data/raw/brick_CFs.xlsx
+++ b/exposan/bwaise/data/raw/brick_CFs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="104">
   <si>
     <t>-</t>
   </si>
@@ -28,6 +28,15 @@
     <t>ReCiPe Endpoint (I,A) (obsolete)</t>
   </si>
   <si>
+    <t>ReCiPe Midpoint (E) V1.13</t>
+  </si>
+  <si>
+    <t>ReCiPe Midpoint (H) V1.13</t>
+  </si>
+  <si>
+    <t>ReCiPe Midpoint (I) V1.13</t>
+  </si>
+  <si>
     <t>TRACI (obsolete)</t>
   </si>
   <si>
@@ -43,61 +52,151 @@
     <t>total</t>
   </si>
   <si>
+    <t>agricultural land occupation</t>
+  </si>
+  <si>
+    <t>climate change</t>
+  </si>
+  <si>
+    <t>fossil depletion</t>
+  </si>
+  <si>
+    <t>freshwater ecotoxicity</t>
+  </si>
+  <si>
+    <t>freshwater eutrophication</t>
+  </si>
+  <si>
+    <t>human toxicity</t>
+  </si>
+  <si>
+    <t>ionising radiation</t>
+  </si>
+  <si>
+    <t>marine ecotoxicity</t>
+  </si>
+  <si>
+    <t>marine eutrophication</t>
+  </si>
+  <si>
+    <t>metal depletion</t>
+  </si>
+  <si>
+    <t>natural land transformation</t>
+  </si>
+  <si>
+    <t>ozone depletion</t>
+  </si>
+  <si>
+    <t>particulate matter formation</t>
+  </si>
+  <si>
+    <t>photochemical oxidant formation</t>
+  </si>
+  <si>
+    <t>terrestrial acidification</t>
+  </si>
+  <si>
+    <t>terrestrial ecotoxicity</t>
+  </si>
+  <si>
+    <t>urban land occupation</t>
+  </si>
+  <si>
+    <t>water depletion</t>
+  </si>
+  <si>
     <t>environmental impact</t>
   </si>
   <si>
     <t>activity functional unit</t>
   </si>
   <si>
-    <t>agricultural land occupation</t>
-  </si>
-  <si>
     <t>climate change, ecosystems</t>
   </si>
   <si>
-    <t>freshwater ecotoxicity</t>
-  </si>
-  <si>
-    <t>freshwater eutrophication</t>
-  </si>
-  <si>
-    <t>marine ecotoxicity</t>
-  </si>
-  <si>
-    <t>natural land transformation</t>
-  </si>
-  <si>
-    <t>terrestrial acidification</t>
-  </si>
-  <si>
-    <t>terrestrial ecotoxicity</t>
-  </si>
-  <si>
-    <t>urban land occupation</t>
-  </si>
-  <si>
     <t>climate change, human health</t>
   </si>
   <si>
-    <t>human toxicity</t>
-  </si>
-  <si>
-    <t>ionising radiation</t>
-  </si>
-  <si>
-    <t>ozone depletion</t>
-  </si>
-  <si>
-    <t>particulate matter formation</t>
-  </si>
-  <si>
-    <t>photochemical oxidant formation</t>
-  </si>
-  <si>
-    <t>fossil depletion</t>
-  </si>
-  <si>
-    <t>metal depletion</t>
+    <t>ALOP</t>
+  </si>
+  <si>
+    <t>GWP500</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>FETPinf</t>
+  </si>
+  <si>
+    <t>FEP</t>
+  </si>
+  <si>
+    <t>HTPinf</t>
+  </si>
+  <si>
+    <t>IRP_HE</t>
+  </si>
+  <si>
+    <t>METPinf</t>
+  </si>
+  <si>
+    <t>MEP</t>
+  </si>
+  <si>
+    <t>MDP</t>
+  </si>
+  <si>
+    <t>NLTP</t>
+  </si>
+  <si>
+    <t>ODPinf</t>
+  </si>
+  <si>
+    <t>PMFP</t>
+  </si>
+  <si>
+    <t>POFP</t>
+  </si>
+  <si>
+    <t>TAP500</t>
+  </si>
+  <si>
+    <t>TETPinf</t>
+  </si>
+  <si>
+    <t>ULOP</t>
+  </si>
+  <si>
+    <t>WDP</t>
+  </si>
+  <si>
+    <t>GWP100</t>
+  </si>
+  <si>
+    <t>TAP100</t>
+  </si>
+  <si>
+    <t>GWP20</t>
+  </si>
+  <si>
+    <t>FETP100</t>
+  </si>
+  <si>
+    <t>HTP100</t>
+  </si>
+  <si>
+    <t>IRP_I</t>
+  </si>
+  <si>
+    <t>METP100</t>
+  </si>
+  <si>
+    <t>TAP20</t>
+  </si>
+  <si>
+    <t>TETP100</t>
   </si>
   <si>
     <t>acidification</t>
@@ -163,6 +262,51 @@
     <t>points</t>
   </si>
   <si>
+    <t>square meter-year</t>
+  </si>
+  <si>
+    <t>kg CO2-Eq</t>
+  </si>
+  <si>
+    <t>kg oil-Eq</t>
+  </si>
+  <si>
+    <t>kg 1,4-DC.</t>
+  </si>
+  <si>
+    <t>kg P-Eq</t>
+  </si>
+  <si>
+    <t>kg U235-Eq</t>
+  </si>
+  <si>
+    <t>kg N-Eq</t>
+  </si>
+  <si>
+    <t>kg Fe-Eq</t>
+  </si>
+  <si>
+    <t>square meter</t>
+  </si>
+  <si>
+    <t>kg CFC-11.</t>
+  </si>
+  <si>
+    <t>kg PM10-Eq</t>
+  </si>
+  <si>
+    <t>kg NMVOC-.</t>
+  </si>
+  <si>
+    <t>kg SO2-Eq</t>
+  </si>
+  <si>
+    <t>m3 water-.</t>
+  </si>
+  <si>
+    <t>kg 1,4-DB.</t>
+  </si>
+  <si>
     <t>moles of .</t>
   </si>
   <si>
@@ -170,12 +314,6 @@
   </si>
   <si>
     <t>kg N</t>
-  </si>
-  <si>
-    <t>kg CO2-Eq</t>
-  </si>
-  <si>
-    <t>kg CFC-11.</t>
   </si>
   <si>
     <t>kg NOx-Eq</t>
@@ -545,13 +683,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BV15"/>
+  <dimension ref="A1:DX15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:74">
+    <row r="1" spans="1:128">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -636,14 +774,74 @@
       <c r="BT1" s="1"/>
       <c r="BU1" s="1"/>
       <c r="BV1" s="1"/>
+      <c r="BW1" s="1"/>
+      <c r="BX1" s="1"/>
+      <c r="BY1" s="1"/>
+      <c r="BZ1" s="1"/>
+      <c r="CA1" s="1"/>
+      <c r="CB1" s="1"/>
+      <c r="CC1" s="1"/>
+      <c r="CD1" s="1"/>
+      <c r="CE1" s="1"/>
+      <c r="CF1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="CG1" s="1"/>
+      <c r="CH1" s="1"/>
+      <c r="CI1" s="1"/>
+      <c r="CJ1" s="1"/>
+      <c r="CK1" s="1"/>
+      <c r="CL1" s="1"/>
+      <c r="CM1" s="1"/>
+      <c r="CN1" s="1"/>
+      <c r="CO1" s="1"/>
+      <c r="CP1" s="1"/>
+      <c r="CQ1" s="1"/>
+      <c r="CR1" s="1"/>
+      <c r="CS1" s="1"/>
+      <c r="CT1" s="1"/>
+      <c r="CU1" s="1"/>
+      <c r="CV1" s="1"/>
+      <c r="CW1" s="1"/>
+      <c r="CX1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
+      <c r="DB1" s="1"/>
+      <c r="DC1" s="1"/>
+      <c r="DD1" s="1"/>
+      <c r="DE1" s="1"/>
+      <c r="DF1" s="1"/>
+      <c r="DG1" s="1"/>
+      <c r="DH1" s="1"/>
+      <c r="DI1" s="1"/>
+      <c r="DJ1" s="1"/>
+      <c r="DK1" s="1"/>
+      <c r="DL1" s="1"/>
+      <c r="DM1" s="1"/>
+      <c r="DN1" s="1"/>
+      <c r="DO1" s="1"/>
+      <c r="DP1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DQ1" s="1"/>
+      <c r="DR1" s="1"/>
+      <c r="DS1" s="1"/>
+      <c r="DT1" s="1"/>
+      <c r="DU1" s="1"/>
+      <c r="DV1" s="1"/>
+      <c r="DW1" s="1"/>
+      <c r="DX1" s="1"/>
     </row>
-    <row r="2" spans="1:74">
+    <row r="2" spans="1:128">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -655,7 +853,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -664,15 +862,15 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
@@ -684,7 +882,7 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
@@ -693,15 +891,15 @@
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="AT2" s="1"/>
       <c r="AU2" s="1"/>
@@ -713,7 +911,7 @@
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
       <c r="BC2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BD2" s="1"/>
       <c r="BE2" s="1"/>
@@ -722,70 +920,232 @@
       <c r="BH2" s="1"/>
       <c r="BI2" s="1"/>
       <c r="BJ2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
       <c r="BM2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BN2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BQ2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BR2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BS2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BT2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BU2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BV2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BW2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BX2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BY2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BZ2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="CA2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="CB2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CC2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="CD2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="CE2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CF2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="CG2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="CH2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CI2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="CJ2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="CK2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="CL2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="CM2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="CN2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="CO2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="CQ2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="CR2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="CS2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="CT2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CU2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="CV2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="CW2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CX2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="CY2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="CZ2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="DA2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="DB2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="DC2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="DD2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="DE2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="DF2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="DG2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="DH2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="DI2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DJ2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="DK2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="DL2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="DM2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="DN2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="DO2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DP2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="DQ2" s="1"/>
+      <c r="DR2" s="1"/>
+      <c r="DS2" s="1"/>
+      <c r="DT2" s="1"/>
+      <c r="DU2" s="1"/>
+      <c r="DV2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="BO2" s="1"/>
-      <c r="BP2" s="1"/>
-      <c r="BQ2" s="1"/>
-      <c r="BR2" s="1"/>
-      <c r="BS2" s="1"/>
-      <c r="BT2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BU2" s="1"/>
-      <c r="BV2" s="1"/>
+      <c r="DW2" s="1"/>
+      <c r="DX2" s="1"/>
     </row>
-    <row r="3" spans="1:74">
+    <row r="3" spans="1:128">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>23</v>
@@ -797,58 +1157,58 @@
         <v>25</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="T3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="X3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="AK3" s="1" t="s">
         <v>23</v>
@@ -860,58 +1220,58 @@
         <v>25</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AO3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AQ3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS3" s="1" t="s">
+      <c r="BA3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AT3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY3" s="1" t="s">
+      <c r="BB3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AZ3" s="1" t="s">
+      <c r="BE3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="BC3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="BD3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BE3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="BF3" s="1" t="s">
         <v>23</v>
@@ -923,278 +1283,602 @@
         <v>25</v>
       </c>
       <c r="BI3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BJ3" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="BK3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="BL3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BM3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BN3" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="BO3" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="BP3" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="BQ3" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="BR3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BS3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BU3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BV3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BW3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BX3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BY3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BZ3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="CA3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="CB3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="CC3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="CD3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="CE3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="CF3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="CG3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="CH3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CJ3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="CK3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="CL3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="CM3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="CN3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CO3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="CP3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="CQ3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="CR3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="CS3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="CT3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CU3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="CV3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="CW3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="CX3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="CY3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="CZ3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="DB3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="DC3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="DD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="DE3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="DF3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DG3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="DH3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="DI3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="DJ3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="DK3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="DL3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="DM3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="DN3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="DO3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="DP3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="DQ3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="DR3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="DS3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="DT3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="BS3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="BT3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BU3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="BV3" s="1" t="s">
-        <v>35</v>
+      <c r="DU3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="DV3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="DW3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="DX3" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:74">
+    <row r="5" spans="1:128">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="M5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="O5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="P5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="Q5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="R5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="S5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="T5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="U5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="V5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="W5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="X5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="Y5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="Z5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AA5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AB5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AC5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AD5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AE5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AF5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AG5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AH5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AI5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AJ5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AK5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AL5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AM5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AN5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AO5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AP5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AQ5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AR5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AS5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AT5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AU5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AV5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AW5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AX5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AY5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="AZ5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BA5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BB5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BC5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BD5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BE5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BF5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BG5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BH5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BI5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BJ5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BK5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BL5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BM5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="BN5" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="BO5" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="BP5" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="BQ5" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="BR5" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="BS5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="BT5" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="BU5" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="BV5" t="s">
-        <v>57</v>
+        <v>88</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>89</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>90</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>92</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB5" t="s">
+        <v>94</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>85</v>
+      </c>
+      <c r="CD5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE5" t="s">
+        <v>95</v>
+      </c>
+      <c r="CF5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG5" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH5" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>85</v>
+      </c>
+      <c r="CJ5" t="s">
+        <v>86</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>85</v>
+      </c>
+      <c r="CL5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>96</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>88</v>
+      </c>
+      <c r="CO5" t="s">
+        <v>89</v>
+      </c>
+      <c r="CP5" t="s">
+        <v>90</v>
+      </c>
+      <c r="CQ5" t="s">
+        <v>91</v>
+      </c>
+      <c r="CR5" t="s">
+        <v>92</v>
+      </c>
+      <c r="CS5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT5" t="s">
+        <v>94</v>
+      </c>
+      <c r="CU5" t="s">
+        <v>85</v>
+      </c>
+      <c r="CV5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CW5" t="s">
+        <v>95</v>
+      </c>
+      <c r="CX5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CY5" t="s">
+        <v>83</v>
+      </c>
+      <c r="CZ5" t="s">
+        <v>84</v>
+      </c>
+      <c r="DA5" t="s">
+        <v>85</v>
+      </c>
+      <c r="DB5" t="s">
+        <v>86</v>
+      </c>
+      <c r="DC5" t="s">
+        <v>85</v>
+      </c>
+      <c r="DD5" t="s">
+        <v>87</v>
+      </c>
+      <c r="DE5" t="s">
+        <v>85</v>
+      </c>
+      <c r="DF5" t="s">
+        <v>88</v>
+      </c>
+      <c r="DG5" t="s">
+        <v>89</v>
+      </c>
+      <c r="DH5" t="s">
+        <v>90</v>
+      </c>
+      <c r="DI5" t="s">
+        <v>91</v>
+      </c>
+      <c r="DJ5" t="s">
+        <v>92</v>
+      </c>
+      <c r="DK5" t="s">
+        <v>93</v>
+      </c>
+      <c r="DL5" t="s">
+        <v>94</v>
+      </c>
+      <c r="DM5" t="s">
+        <v>85</v>
+      </c>
+      <c r="DN5" t="s">
+        <v>82</v>
+      </c>
+      <c r="DO5" t="s">
+        <v>95</v>
+      </c>
+      <c r="DP5" t="s">
+        <v>97</v>
+      </c>
+      <c r="DQ5" t="s">
+        <v>98</v>
+      </c>
+      <c r="DR5" t="s">
+        <v>99</v>
+      </c>
+      <c r="DS5" t="s">
+        <v>83</v>
+      </c>
+      <c r="DT5" t="s">
+        <v>91</v>
+      </c>
+      <c r="DU5" t="s">
+        <v>100</v>
+      </c>
+      <c r="DV5" t="s">
+        <v>101</v>
+      </c>
+      <c r="DW5" t="s">
+        <v>102</v>
+      </c>
+      <c r="DX5" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="1:128">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>8.794086995884491E-05</v>
@@ -1386,39 +2070,201 @@
         <v>0.07486540224893615</v>
       </c>
       <c r="BN6">
+        <v>0.0103861725410803</v>
+      </c>
+      <c r="BO6">
+        <v>0.2303993012359031</v>
+      </c>
+      <c r="BP6">
+        <v>0.09476535464792518</v>
+      </c>
+      <c r="BQ6">
+        <v>0.003236448064663434</v>
+      </c>
+      <c r="BR6">
+        <v>4.727122161727755E-05</v>
+      </c>
+      <c r="BS6">
+        <v>2.661986733470272</v>
+      </c>
+      <c r="BT6">
+        <v>0.0167005896305158</v>
+      </c>
+      <c r="BU6">
+        <v>2.862139662520828</v>
+      </c>
+      <c r="BV6">
+        <v>4.064369478743542E-05</v>
+      </c>
+      <c r="BW6">
+        <v>0.4444255056402289</v>
+      </c>
+      <c r="BX6">
+        <v>-6.599659638227842E-05</v>
+      </c>
+      <c r="BY6">
+        <v>2.408272394351298E-08</v>
+      </c>
+      <c r="BZ6">
+        <v>0.0004472161409278899</v>
+      </c>
+      <c r="CA6">
+        <v>0.0008886342528222678</v>
+      </c>
+      <c r="CB6">
+        <v>0.000881757370536982</v>
+      </c>
+      <c r="CC6">
+        <v>0.0003114081835497947</v>
+      </c>
+      <c r="CD6">
+        <v>0.0138738478515481</v>
+      </c>
+      <c r="CE6">
+        <v>0.0007311441066935041</v>
+      </c>
+      <c r="CF6">
+        <v>0.0103861725410803</v>
+      </c>
+      <c r="CG6">
+        <v>0.2404383094681986</v>
+      </c>
+      <c r="CH6">
+        <v>0.09476535464792518</v>
+      </c>
+      <c r="CI6">
+        <v>0.003202800702504194</v>
+      </c>
+      <c r="CJ6">
+        <v>4.727122161727755E-05</v>
+      </c>
+      <c r="CK6">
+        <v>0.05214474622516788</v>
+      </c>
+      <c r="CL6">
+        <v>0.0167005896305158</v>
+      </c>
+      <c r="CM6">
+        <v>0.002976633871396917</v>
+      </c>
+      <c r="CN6">
+        <v>4.064369478743542E-05</v>
+      </c>
+      <c r="CO6">
+        <v>0.4444255056402289</v>
+      </c>
+      <c r="CP6">
+        <v>-6.599659638227842E-05</v>
+      </c>
+      <c r="CQ6">
+        <v>2.408272394351298E-08</v>
+      </c>
+      <c r="CR6">
+        <v>0.0004472161409278899</v>
+      </c>
+      <c r="CS6">
+        <v>0.0008886342528222678</v>
+      </c>
+      <c r="CT6">
+        <v>0.0007746566817744609</v>
+      </c>
+      <c r="CU6">
+        <v>3.362361766324114E-05</v>
+      </c>
+      <c r="CV6">
+        <v>0.0138738478515481</v>
+      </c>
+      <c r="CW6">
+        <v>0.0007311441066935041</v>
+      </c>
+      <c r="CX6">
+        <v>0.0103861725410803</v>
+      </c>
+      <c r="CY6">
+        <v>0.2654121962534866</v>
+      </c>
+      <c r="CZ6">
+        <v>0.09476535464792518</v>
+      </c>
+      <c r="DA6">
+        <v>0.003202785434692088</v>
+      </c>
+      <c r="DB6">
+        <v>4.727122161727755E-05</v>
+      </c>
+      <c r="DC6">
+        <v>0.008587188169044191</v>
+      </c>
+      <c r="DD6">
+        <v>0.008587751381441256</v>
+      </c>
+      <c r="DE6">
+        <v>0.001944452064534172</v>
+      </c>
+      <c r="DF6">
+        <v>4.064369478743542E-05</v>
+      </c>
+      <c r="DG6">
+        <v>0.4444255056402289</v>
+      </c>
+      <c r="DH6">
+        <v>-6.599659638227842E-05</v>
+      </c>
+      <c r="DI6">
+        <v>2.408272394351298E-08</v>
+      </c>
+      <c r="DJ6">
+        <v>0.0004472161409278899</v>
+      </c>
+      <c r="DK6">
+        <v>0.0008886342528222678</v>
+      </c>
+      <c r="DL6">
+        <v>0.0007231859221111943</v>
+      </c>
+      <c r="DM6">
+        <v>3.361496970664196E-05</v>
+      </c>
+      <c r="DN6">
+        <v>0.0138738478515481</v>
+      </c>
+      <c r="DO6">
+        <v>0.0007311441066935041</v>
+      </c>
+      <c r="DP6">
         <v>0.04805428994690507</v>
       </c>
-      <c r="BO6">
+      <c r="DQ6">
         <v>0.07837245744876468</v>
       </c>
-      <c r="BP6">
+      <c r="DR6">
         <v>5.604505750703527E-05</v>
       </c>
-      <c r="BQ6">
+      <c r="DS6">
         <v>0.2397801527101718</v>
       </c>
-      <c r="BR6">
+      <c r="DT6">
         <v>2.434275991396352E-08</v>
       </c>
-      <c r="BS6">
+      <c r="DU6">
         <v>0.0007144928219773217</v>
       </c>
-      <c r="BT6">
+      <c r="DV6">
         <v>0.0001945670170407161</v>
       </c>
-      <c r="BU6">
+      <c r="DW6">
         <v>3.39294149185398</v>
       </c>
-      <c r="BV6">
+      <c r="DX6">
         <v>0.0002765229783001658</v>
       </c>
     </row>
-    <row r="7" spans="1:74">
+    <row r="7" spans="1:128">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <v>0.000171027487122567</v>
@@ -1610,39 +2456,201 @@
         <v>0.03027757387073565</v>
       </c>
       <c r="BN7">
+        <v>0.008299501475556229</v>
+      </c>
+      <c r="BO7">
+        <v>0.3037820228453487</v>
+      </c>
+      <c r="BP7">
+        <v>0.0870638127422714</v>
+      </c>
+      <c r="BQ7">
+        <v>0.003800712039034528</v>
+      </c>
+      <c r="BR7">
+        <v>3.640757395505466E-05</v>
+      </c>
+      <c r="BS7">
+        <v>1.984829426425822</v>
+      </c>
+      <c r="BT7">
+        <v>0.01302354699155258</v>
+      </c>
+      <c r="BU7">
+        <v>2.282392259297031</v>
+      </c>
+      <c r="BV7">
+        <v>4.443423334258444E-05</v>
+      </c>
+      <c r="BW7">
+        <v>0.01193802333624145</v>
+      </c>
+      <c r="BX7">
+        <v>-2.655335691774185E-05</v>
+      </c>
+      <c r="BY7">
+        <v>2.546336698418853E-08</v>
+      </c>
+      <c r="BZ7">
+        <v>0.0004043123438355056</v>
+      </c>
+      <c r="CA7">
+        <v>0.001123138666205846</v>
+      </c>
+      <c r="CB7">
+        <v>0.0009852200664350371</v>
+      </c>
+      <c r="CC7">
+        <v>0.0003216494406756548</v>
+      </c>
+      <c r="CD7">
+        <v>0.0130779363767336</v>
+      </c>
+      <c r="CE7">
+        <v>0.0005479313179918572</v>
+      </c>
+      <c r="CF7">
+        <v>0.008299501475556229</v>
+      </c>
+      <c r="CG7">
+        <v>0.3107135337607931</v>
+      </c>
+      <c r="CH7">
+        <v>0.0870638127422714</v>
+      </c>
+      <c r="CI7">
+        <v>0.003765775136835688</v>
+      </c>
+      <c r="CJ7">
+        <v>3.640757395505466E-05</v>
+      </c>
+      <c r="CK7">
+        <v>0.0486597849395642</v>
+      </c>
+      <c r="CL7">
+        <v>0.01302354699155258</v>
+      </c>
+      <c r="CM7">
+        <v>0.00331075562144972</v>
+      </c>
+      <c r="CN7">
+        <v>4.443423334258444E-05</v>
+      </c>
+      <c r="CO7">
+        <v>0.01193802333624145</v>
+      </c>
+      <c r="CP7">
+        <v>-2.655335691774185E-05</v>
+      </c>
+      <c r="CQ7">
+        <v>2.546336698418853E-08</v>
+      </c>
+      <c r="CR7">
+        <v>0.0004043123438355056</v>
+      </c>
+      <c r="CS7">
+        <v>0.001123138666205846</v>
+      </c>
+      <c r="CT7">
+        <v>0.0008567253163213728</v>
+      </c>
+      <c r="CU7">
+        <v>3.660031952608049E-05</v>
+      </c>
+      <c r="CV7">
+        <v>0.0130779363767336</v>
+      </c>
+      <c r="CW7">
+        <v>0.0005479313179918572</v>
+      </c>
+      <c r="CX7">
+        <v>0.008299501475556229</v>
+      </c>
+      <c r="CY7">
+        <v>0.3282190020151859</v>
+      </c>
+      <c r="CZ7">
+        <v>0.0870638127422714</v>
+      </c>
+      <c r="DA7">
+        <v>0.003765763087197824</v>
+      </c>
+      <c r="DB7">
+        <v>3.640757395505466E-05</v>
+      </c>
+      <c r="DC7">
+        <v>0.01327074810541124</v>
+      </c>
+      <c r="DD7">
+        <v>0.005435970316126508</v>
+      </c>
+      <c r="DE7">
+        <v>0.001820620423778571</v>
+      </c>
+      <c r="DF7">
+        <v>4.443423334258444E-05</v>
+      </c>
+      <c r="DG7">
+        <v>0.01193802333624145</v>
+      </c>
+      <c r="DH7">
+        <v>-2.655335691774185E-05</v>
+      </c>
+      <c r="DI7">
+        <v>2.546336698418853E-08</v>
+      </c>
+      <c r="DJ7">
+        <v>0.0004043123438355056</v>
+      </c>
+      <c r="DK7">
+        <v>0.001123138666205846</v>
+      </c>
+      <c r="DL7">
+        <v>0.0007942365290417057</v>
+      </c>
+      <c r="DM7">
+        <v>3.659447377067793E-05</v>
+      </c>
+      <c r="DN7">
+        <v>0.0130779363767336</v>
+      </c>
+      <c r="DO7">
+        <v>0.0005479313179918572</v>
+      </c>
+      <c r="DP7">
         <v>0.05474950226926532</v>
       </c>
-      <c r="BO7">
+      <c r="DQ7">
         <v>0.06640011204675106</v>
       </c>
-      <c r="BP7">
+      <c r="DR7">
         <v>6.958058239052774E-05</v>
       </c>
-      <c r="BQ7">
+      <c r="DS7">
         <v>0.3110112622277846</v>
       </c>
-      <c r="BR7">
+      <c r="DT7">
         <v>2.556203827466724E-08</v>
       </c>
-      <c r="BS7">
+      <c r="DU7">
         <v>0.0008795405319527763</v>
       </c>
-      <c r="BT7">
+      <c r="DV7">
         <v>0.0001881737052007664</v>
       </c>
-      <c r="BU7">
+      <c r="DW7">
         <v>3.42555342425865</v>
       </c>
-      <c r="BV7">
+      <c r="DX7">
         <v>0.0002266921335745087</v>
       </c>
     </row>
-    <row r="8" spans="1:74">
+    <row r="8" spans="1:128">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>0.0004350765840229042</v>
@@ -1834,39 +2842,201 @@
         <v>0.01643731931489504</v>
       </c>
       <c r="BN8">
+        <v>0.02760429068529268</v>
+      </c>
+      <c r="BO8">
+        <v>0.1776326049121358</v>
+      </c>
+      <c r="BP8">
+        <v>0.03468947752728003</v>
+      </c>
+      <c r="BQ8">
+        <v>0.001995995699355791</v>
+      </c>
+      <c r="BR8">
+        <v>2.242801671300862E-05</v>
+      </c>
+      <c r="BS8">
+        <v>1.186019953611035</v>
+      </c>
+      <c r="BT8">
+        <v>0.006944878799651908</v>
+      </c>
+      <c r="BU8">
+        <v>1.489505848741268</v>
+      </c>
+      <c r="BV8">
+        <v>2.98277811090804E-05</v>
+      </c>
+      <c r="BW8">
+        <v>0.00909551972546039</v>
+      </c>
+      <c r="BX8">
+        <v>-2.596205558573115E-05</v>
+      </c>
+      <c r="BY8">
+        <v>1.232173546664105E-08</v>
+      </c>
+      <c r="BZ8">
+        <v>0.00027400028201456</v>
+      </c>
+      <c r="CA8">
+        <v>0.0005929368386987813</v>
+      </c>
+      <c r="CB8">
+        <v>0.0006718464461157507</v>
+      </c>
+      <c r="CC8">
+        <v>0.00019458284151007</v>
+      </c>
+      <c r="CD8">
+        <v>0.005805102509820544</v>
+      </c>
+      <c r="CE8">
+        <v>0.0004997311308663114</v>
+      </c>
+      <c r="CF8">
+        <v>0.02760429068529268</v>
+      </c>
+      <c r="CG8">
+        <v>0.1820698956301594</v>
+      </c>
+      <c r="CH8">
+        <v>0.03468947752728003</v>
+      </c>
+      <c r="CI8">
+        <v>0.001971053828459281</v>
+      </c>
+      <c r="CJ8">
+        <v>2.242801671300862E-05</v>
+      </c>
+      <c r="CK8">
+        <v>0.02861257890517663</v>
+      </c>
+      <c r="CL8">
+        <v>0.006944878799651908</v>
+      </c>
+      <c r="CM8">
+        <v>0.001857149342305228</v>
+      </c>
+      <c r="CN8">
+        <v>2.98277811090804E-05</v>
+      </c>
+      <c r="CO8">
+        <v>0.00909551972546039</v>
+      </c>
+      <c r="CP8">
+        <v>-2.596205558573115E-05</v>
+      </c>
+      <c r="CQ8">
+        <v>1.232173546664105E-08</v>
+      </c>
+      <c r="CR8">
+        <v>0.00027400028201456</v>
+      </c>
+      <c r="CS8">
+        <v>0.0005929368386987813</v>
+      </c>
+      <c r="CT8">
+        <v>0.0005995374007521057</v>
+      </c>
+      <c r="CU8">
+        <v>2.095864906603725E-05</v>
+      </c>
+      <c r="CV8">
+        <v>0.005805102509820544</v>
+      </c>
+      <c r="CW8">
+        <v>0.0004997311308663114</v>
+      </c>
+      <c r="CX8">
+        <v>0.02760429068529268</v>
+      </c>
+      <c r="CY8">
+        <v>0.1930921699370149</v>
+      </c>
+      <c r="CZ8">
+        <v>0.03468947752728003</v>
+      </c>
+      <c r="DA8">
+        <v>0.001971046259825754</v>
+      </c>
+      <c r="DB8">
+        <v>2.242801671300862E-05</v>
+      </c>
+      <c r="DC8">
+        <v>0.005083275575803493</v>
+      </c>
+      <c r="DD8">
+        <v>0.002513127448020427</v>
+      </c>
+      <c r="DE8">
+        <v>0.001072562475158656</v>
+      </c>
+      <c r="DF8">
+        <v>2.98277811090804E-05</v>
+      </c>
+      <c r="DG8">
+        <v>0.00909551972546039</v>
+      </c>
+      <c r="DH8">
+        <v>-2.596205558573115E-05</v>
+      </c>
+      <c r="DI8">
+        <v>1.232173546664105E-08</v>
+      </c>
+      <c r="DJ8">
+        <v>0.00027400028201456</v>
+      </c>
+      <c r="DK8">
+        <v>0.0005929368386987813</v>
+      </c>
+      <c r="DL8">
+        <v>0.0005642242761222568</v>
+      </c>
+      <c r="DM8">
+        <v>2.095467157745979E-05</v>
+      </c>
+      <c r="DN8">
+        <v>0.005805102509820544</v>
+      </c>
+      <c r="DO8">
+        <v>0.0004997311308663114</v>
+      </c>
+      <c r="DP8">
         <v>0.03631571441567157</v>
       </c>
-      <c r="BO8">
+      <c r="DQ8">
         <v>0.08151795844422337</v>
       </c>
-      <c r="BP8">
+      <c r="DR8">
         <v>4.199754743280298E-05</v>
       </c>
-      <c r="BQ8">
+      <c r="DS8">
         <v>0.1826126440602099</v>
       </c>
-      <c r="BR8">
+      <c r="DT8">
         <v>1.231390307881854E-08</v>
       </c>
-      <c r="BS8">
+      <c r="DU8">
         <v>0.0004793745743702594</v>
       </c>
-      <c r="BT8">
+      <c r="DV8">
         <v>0.0001901071348833808</v>
       </c>
-      <c r="BU8">
+      <c r="DW8">
         <v>1.777357055323549</v>
       </c>
-      <c r="BV8">
+      <c r="DX8">
         <v>0.0001623095685052265</v>
       </c>
     </row>
-    <row r="9" spans="1:74">
+    <row r="9" spans="1:128">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>0.003467084616428644</v>
@@ -2058,39 +3228,201 @@
         <v>0.02415126486282889</v>
       </c>
       <c r="BN9">
+        <v>0.02357196109062761</v>
+      </c>
+      <c r="BO9">
+        <v>0.1522737240673726</v>
+      </c>
+      <c r="BP9">
+        <v>0.06488727104932324</v>
+      </c>
+      <c r="BQ9">
+        <v>0.003265849920549914</v>
+      </c>
+      <c r="BR9">
+        <v>2.03673533384744E-05</v>
+      </c>
+      <c r="BS9">
+        <v>1.366105064602259</v>
+      </c>
+      <c r="BT9">
+        <v>0.007467567139748909</v>
+      </c>
+      <c r="BU9">
+        <v>1.823903551214215</v>
+      </c>
+      <c r="BV9">
+        <v>8.879599219563351E-05</v>
+      </c>
+      <c r="BW9">
+        <v>0.01433404165816363</v>
+      </c>
+      <c r="BX9">
+        <v>-2.871850797399322E-05</v>
+      </c>
+      <c r="BY9">
+        <v>1.928909261312501E-08</v>
+      </c>
+      <c r="BZ9">
+        <v>0.0002598237301294781</v>
+      </c>
+      <c r="CA9">
+        <v>0.0006737006631758199</v>
+      </c>
+      <c r="CB9">
+        <v>0.0006310552854680861</v>
+      </c>
+      <c r="CC9">
+        <v>0.0003657654788371678</v>
+      </c>
+      <c r="CD9">
+        <v>0.008905585545384048</v>
+      </c>
+      <c r="CE9">
+        <v>0.003075877574241802</v>
+      </c>
+      <c r="CF9">
+        <v>0.02357196109062761</v>
+      </c>
+      <c r="CG9">
+        <v>0.1615156981500135</v>
+      </c>
+      <c r="CH9">
+        <v>0.06488727104932324</v>
+      </c>
+      <c r="CI9">
+        <v>0.003233503989349029</v>
+      </c>
+      <c r="CJ9">
+        <v>2.03673533384744E-05</v>
+      </c>
+      <c r="CK9">
+        <v>0.0316690572714555</v>
+      </c>
+      <c r="CL9">
+        <v>0.007467567139748909</v>
+      </c>
+      <c r="CM9">
+        <v>0.002891742637576801</v>
+      </c>
+      <c r="CN9">
+        <v>8.879599219563351E-05</v>
+      </c>
+      <c r="CO9">
+        <v>0.01433404165816363</v>
+      </c>
+      <c r="CP9">
+        <v>-2.871850797399322E-05</v>
+      </c>
+      <c r="CQ9">
+        <v>1.928909261312501E-08</v>
+      </c>
+      <c r="CR9">
+        <v>0.0002598237301294781</v>
+      </c>
+      <c r="CS9">
+        <v>0.0006737006631758199</v>
+      </c>
+      <c r="CT9">
+        <v>0.0005430101588594997</v>
+      </c>
+      <c r="CU9">
+        <v>9.619439367267181E-05</v>
+      </c>
+      <c r="CV9">
+        <v>0.008905585545384048</v>
+      </c>
+      <c r="CW9">
+        <v>0.003075877574241802</v>
+      </c>
+      <c r="CX9">
+        <v>0.02357196109062761</v>
+      </c>
+      <c r="CY9">
+        <v>0.1831091924769379</v>
+      </c>
+      <c r="CZ9">
+        <v>0.06488727104932324</v>
+      </c>
+      <c r="DA9">
+        <v>0.003233274130506589</v>
+      </c>
+      <c r="DB9">
+        <v>2.03673533384744E-05</v>
+      </c>
+      <c r="DC9">
+        <v>0.00803556349558222</v>
+      </c>
+      <c r="DD9">
+        <v>0.002663271594462145</v>
+      </c>
+      <c r="DE9">
+        <v>0.001538228594680506</v>
+      </c>
+      <c r="DF9">
+        <v>8.879599219563351E-05</v>
+      </c>
+      <c r="DG9">
+        <v>0.01433404165816363</v>
+      </c>
+      <c r="DH9">
+        <v>-2.871850797399322E-05</v>
+      </c>
+      <c r="DI9">
+        <v>1.928909261312501E-08</v>
+      </c>
+      <c r="DJ9">
+        <v>0.0002598237301294781</v>
+      </c>
+      <c r="DK9">
+        <v>0.0006737006631758199</v>
+      </c>
+      <c r="DL9">
+        <v>0.0004957490881509317</v>
+      </c>
+      <c r="DM9">
+        <v>9.602320375535798E-05</v>
+      </c>
+      <c r="DN9">
+        <v>0.008905585545384048</v>
+      </c>
+      <c r="DO9">
+        <v>0.003075877574241802</v>
+      </c>
+      <c r="DP9">
         <v>0.03317558357476476</v>
       </c>
-      <c r="BO9">
+      <c r="DQ9">
         <v>0.05232921026551538</v>
       </c>
-      <c r="BP9">
+      <c r="DR9">
         <v>5.94298643879249E-05</v>
       </c>
-      <c r="BQ9">
+      <c r="DS9">
         <v>0.1611537143473335</v>
       </c>
-      <c r="BR9">
+      <c r="DT9">
         <v>1.94287116776855E-08</v>
       </c>
-      <c r="BS9">
+      <c r="DU9">
         <v>0.0005321466237066264</v>
       </c>
-      <c r="BT9">
+      <c r="DV9">
         <v>0.0001486447003139852</v>
       </c>
-      <c r="BU9">
+      <c r="DW9">
         <v>3.225664749305578</v>
       </c>
-      <c r="BV9">
+      <c r="DX9">
         <v>0.0001305676793732226</v>
       </c>
     </row>
-    <row r="10" spans="1:74">
+    <row r="10" spans="1:128">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C10">
         <v>-4.737087422568732E-06</v>
@@ -2282,39 +3614,201 @@
         <v>-0.001669285254397156</v>
       </c>
       <c r="BN10">
+        <v>-0.0003270446488158221</v>
+      </c>
+      <c r="BO10">
+        <v>-0.01056987059632261</v>
+      </c>
+      <c r="BP10">
+        <v>-0.004511670588210743</v>
+      </c>
+      <c r="BQ10">
+        <v>-0.0001762330976864171</v>
+      </c>
+      <c r="BR10">
+        <v>-1.101098389793084E-06</v>
+      </c>
+      <c r="BS10">
+        <v>-0.1466322437878562</v>
+      </c>
+      <c r="BT10">
+        <v>-0.0008895961179376972</v>
+      </c>
+      <c r="BU10">
+        <v>-0.1466927762283242</v>
+      </c>
+      <c r="BV10">
+        <v>-3.826712864624188E-06</v>
+      </c>
+      <c r="BW10">
+        <v>-0.0002785289953459669</v>
+      </c>
+      <c r="BX10">
+        <v>1.865919207605458E-06</v>
+      </c>
+      <c r="BY10">
+        <v>-2.103855832934659E-09</v>
+      </c>
+      <c r="BZ10">
+        <v>-0.0001149417839375777</v>
+      </c>
+      <c r="CA10">
+        <v>-0.0001063923087018648</v>
+      </c>
+      <c r="CB10">
+        <v>-8.1804868446291E-05</v>
+      </c>
+      <c r="CC10">
+        <v>-2.506439816637554E-05</v>
+      </c>
+      <c r="CD10">
+        <v>-0.0008303236142377587</v>
+      </c>
+      <c r="CE10">
+        <v>-1.980473941110385E-05</v>
+      </c>
+      <c r="CF10">
+        <v>-0.0003270446488158221</v>
+      </c>
+      <c r="CG10">
+        <v>-0.01079822723412684</v>
+      </c>
+      <c r="CH10">
+        <v>-0.004511670588210743</v>
+      </c>
+      <c r="CI10">
+        <v>-0.0001733398703440877</v>
+      </c>
+      <c r="CJ10">
+        <v>-1.101098389793084E-06</v>
+      </c>
+      <c r="CK10">
+        <v>-0.00599098876921268</v>
+      </c>
+      <c r="CL10">
+        <v>-0.0008895961179376972</v>
+      </c>
+      <c r="CM10">
+        <v>-0.0001714547802201379</v>
+      </c>
+      <c r="CN10">
+        <v>-3.826712864624188E-06</v>
+      </c>
+      <c r="CO10">
+        <v>-0.0002785289953459669</v>
+      </c>
+      <c r="CP10">
+        <v>1.865919207605458E-06</v>
+      </c>
+      <c r="CQ10">
+        <v>-2.103855832934659E-09</v>
+      </c>
+      <c r="CR10">
+        <v>-0.0001149417839375777</v>
+      </c>
+      <c r="CS10">
+        <v>-0.0001063923087018648</v>
+      </c>
+      <c r="CT10">
+        <v>-6.840513900650519E-05</v>
+      </c>
+      <c r="CU10">
+        <v>-2.367861380575093E-06</v>
+      </c>
+      <c r="CV10">
+        <v>-0.0008303236142377587</v>
+      </c>
+      <c r="CW10">
+        <v>-1.980473941110385E-05</v>
+      </c>
+      <c r="CX10">
+        <v>-0.0003270446488158221</v>
+      </c>
+      <c r="CY10">
+        <v>-0.01129320593084418</v>
+      </c>
+      <c r="CZ10">
+        <v>-0.004511670588210743</v>
+      </c>
+      <c r="DA10">
+        <v>-0.0001733389641522415</v>
+      </c>
+      <c r="DB10">
+        <v>-1.101098389793084E-06</v>
+      </c>
+      <c r="DC10">
+        <v>-0.0007515130076101416</v>
+      </c>
+      <c r="DD10">
+        <v>-0.0001934845451453056</v>
+      </c>
+      <c r="DE10">
+        <v>-0.0001133074848265907</v>
+      </c>
+      <c r="DF10">
+        <v>-3.826712864624188E-06</v>
+      </c>
+      <c r="DG10">
+        <v>-0.0002785289953459669</v>
+      </c>
+      <c r="DH10">
+        <v>1.865919207605458E-06</v>
+      </c>
+      <c r="DI10">
+        <v>-2.103855832934659E-09</v>
+      </c>
+      <c r="DJ10">
+        <v>-0.0001149417839375777</v>
+      </c>
+      <c r="DK10">
+        <v>-0.0001063923087018648</v>
+      </c>
+      <c r="DL10">
+        <v>-6.210326375521939E-05</v>
+      </c>
+      <c r="DM10">
+        <v>-2.367664012913562E-06</v>
+      </c>
+      <c r="DN10">
+        <v>-0.0008303236142377587</v>
+      </c>
+      <c r="DO10">
+        <v>-1.980473941110385E-05</v>
+      </c>
+      <c r="DP10">
         <v>-0.004515747049010951</v>
       </c>
-      <c r="BO10">
+      <c r="DQ10">
         <v>-0.00315447096974555</v>
       </c>
-      <c r="BP10">
+      <c r="DR10">
         <v>-7.208915151740853E-06</v>
       </c>
-      <c r="BQ10">
+      <c r="DS10">
         <v>-0.01082660578102564</v>
       </c>
-      <c r="BR10">
+      <c r="DT10">
         <v>-2.108204589064716E-09</v>
       </c>
-      <c r="BS10">
+      <c r="DU10">
         <v>-8.954129970080758E-05</v>
       </c>
-      <c r="BT10">
+      <c r="DV10">
         <v>-7.179249395868318E-06</v>
       </c>
-      <c r="BU10">
+      <c r="DW10">
         <v>-0.2687987176873554</v>
       </c>
-      <c r="BV10">
+      <c r="DX10">
         <v>-3.387592784080466E-05</v>
       </c>
     </row>
-    <row r="11" spans="1:74">
+    <row r="11" spans="1:128">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C11">
         <v>0.0007135978124466756</v>
@@ -2506,39 +4000,201 @@
         <v>0.1238154606128195</v>
       </c>
       <c r="BN11">
+        <v>0.0314988029243552</v>
+      </c>
+      <c r="BO11">
+        <v>0.5553389310745553</v>
+      </c>
+      <c r="BP11">
+        <v>0.1554145592714853</v>
+      </c>
+      <c r="BQ11">
+        <v>0.02655420357129178</v>
+      </c>
+      <c r="BR11">
+        <v>0.0002488511430205342</v>
+      </c>
+      <c r="BS11">
+        <v>13.18602289695679</v>
+      </c>
+      <c r="BT11">
+        <v>0.04670204504936146</v>
+      </c>
+      <c r="BU11">
+        <v>23.67844057981528</v>
+      </c>
+      <c r="BV11">
+        <v>0.0002054034410355788</v>
+      </c>
+      <c r="BW11">
+        <v>0.3250756986400337</v>
+      </c>
+      <c r="BX11">
+        <v>-9.977017557930129E-05</v>
+      </c>
+      <c r="BY11">
+        <v>3.621534406050502E-08</v>
+      </c>
+      <c r="BZ11">
+        <v>0.001381535289399253</v>
+      </c>
+      <c r="CA11">
+        <v>0.002329863568001287</v>
+      </c>
+      <c r="CB11">
+        <v>0.002235144332670227</v>
+      </c>
+      <c r="CC11">
+        <v>0.001214818331517639</v>
+      </c>
+      <c r="CD11">
+        <v>0.04483701949788843</v>
+      </c>
+      <c r="CE11">
+        <v>0.008631071134479874</v>
+      </c>
+      <c r="CF11">
+        <v>0.0314988029243552</v>
+      </c>
+      <c r="CG11">
+        <v>0.5774063070122285</v>
+      </c>
+      <c r="CH11">
+        <v>0.1554145592714853</v>
+      </c>
+      <c r="CI11">
+        <v>0.02646331348788647</v>
+      </c>
+      <c r="CJ11">
+        <v>0.0002488511430205342</v>
+      </c>
+      <c r="CK11">
+        <v>0.2506815087422659</v>
+      </c>
+      <c r="CL11">
+        <v>0.04670204504936146</v>
+      </c>
+      <c r="CM11">
+        <v>0.02463743650433387</v>
+      </c>
+      <c r="CN11">
+        <v>0.0002054034410355788</v>
+      </c>
+      <c r="CO11">
+        <v>0.3250756986400337</v>
+      </c>
+      <c r="CP11">
+        <v>-9.977017557930129E-05</v>
+      </c>
+      <c r="CQ11">
+        <v>3.621534406050502E-08</v>
+      </c>
+      <c r="CR11">
+        <v>0.001381535289399253</v>
+      </c>
+      <c r="CS11">
+        <v>0.002329863568001287</v>
+      </c>
+      <c r="CT11">
+        <v>0.002006332817447511</v>
+      </c>
+      <c r="CU11">
+        <v>0.0002315381533710673</v>
+      </c>
+      <c r="CV11">
+        <v>0.04483701949788843</v>
+      </c>
+      <c r="CW11">
+        <v>0.008631071134479874</v>
+      </c>
+      <c r="CX11">
+        <v>0.0314988029243552</v>
+      </c>
+      <c r="CY11">
+        <v>0.6325824031908578</v>
+      </c>
+      <c r="CZ11">
+        <v>0.1554145592714853</v>
+      </c>
+      <c r="DA11">
+        <v>0.02646323236315593</v>
+      </c>
+      <c r="DB11">
+        <v>0.0002488511430205342</v>
+      </c>
+      <c r="DC11">
+        <v>0.03629858145800273</v>
+      </c>
+      <c r="DD11">
+        <v>0.02647078317277649</v>
+      </c>
+      <c r="DE11">
+        <v>0.01764383089232802</v>
+      </c>
+      <c r="DF11">
+        <v>0.0002054034410355788</v>
+      </c>
+      <c r="DG11">
+        <v>0.3250756986400337</v>
+      </c>
+      <c r="DH11">
+        <v>-9.977017557930129E-05</v>
+      </c>
+      <c r="DI11">
+        <v>3.621534406050502E-08</v>
+      </c>
+      <c r="DJ11">
+        <v>0.001381535289399253</v>
+      </c>
+      <c r="DK11">
+        <v>0.002329863568001287</v>
+      </c>
+      <c r="DL11">
+        <v>0.001891200468116588</v>
+      </c>
+      <c r="DM11">
+        <v>0.0002315101096181764</v>
+      </c>
+      <c r="DN11">
+        <v>0.04483701949788843</v>
+      </c>
+      <c r="DO11">
+        <v>0.008631071134479874</v>
+      </c>
+      <c r="DP11">
         <v>0.1197011458648232</v>
       </c>
-      <c r="BO11">
+      <c r="DQ11">
         <v>0.5026693746178221</v>
       </c>
-      <c r="BP11">
+      <c r="DR11">
         <v>0.0003009713527151938</v>
       </c>
-      <c r="BQ11">
+      <c r="DS11">
         <v>0.5789625500590913</v>
       </c>
-      <c r="BR11">
+      <c r="DT11">
         <v>3.958524011484141E-08</v>
       </c>
-      <c r="BS11">
+      <c r="DU11">
         <v>0.001502224780763798</v>
       </c>
-      <c r="BT11">
+      <c r="DV11">
         <v>0.001538875651449092</v>
       </c>
-      <c r="BU11">
+      <c r="DW11">
         <v>10.11615219276999</v>
       </c>
-      <c r="BV11">
+      <c r="DX11">
         <v>0.0007970328255974815</v>
       </c>
     </row>
-    <row r="12" spans="1:74">
+    <row r="12" spans="1:128">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C12">
         <v>-4.737087422568732E-06</v>
@@ -2730,39 +4386,201 @@
         <v>-0.001669285254397156</v>
       </c>
       <c r="BN12">
+        <v>-0.0003270446488158221</v>
+      </c>
+      <c r="BO12">
+        <v>-0.01056987059632261</v>
+      </c>
+      <c r="BP12">
+        <v>-0.004511670588210743</v>
+      </c>
+      <c r="BQ12">
+        <v>-0.0001762330976864171</v>
+      </c>
+      <c r="BR12">
+        <v>-1.101098389793084E-06</v>
+      </c>
+      <c r="BS12">
+        <v>-0.1466322437878562</v>
+      </c>
+      <c r="BT12">
+        <v>-0.0008895961179376972</v>
+      </c>
+      <c r="BU12">
+        <v>-0.1466927762283242</v>
+      </c>
+      <c r="BV12">
+        <v>-3.826712864624188E-06</v>
+      </c>
+      <c r="BW12">
+        <v>-0.0002785289953459669</v>
+      </c>
+      <c r="BX12">
+        <v>-9.977017557930129E-05</v>
+      </c>
+      <c r="BY12">
+        <v>-2.103855832934659E-09</v>
+      </c>
+      <c r="BZ12">
+        <v>-0.0001149417839375777</v>
+      </c>
+      <c r="CA12">
+        <v>-0.0001063923087018648</v>
+      </c>
+      <c r="CB12">
+        <v>-8.1804868446291E-05</v>
+      </c>
+      <c r="CC12">
+        <v>-2.506439816637554E-05</v>
+      </c>
+      <c r="CD12">
+        <v>-0.0008303236142377587</v>
+      </c>
+      <c r="CE12">
+        <v>-1.980473941110385E-05</v>
+      </c>
+      <c r="CF12">
+        <v>-0.0003270446488158221</v>
+      </c>
+      <c r="CG12">
+        <v>-0.01079822723412684</v>
+      </c>
+      <c r="CH12">
+        <v>-0.004511670588210743</v>
+      </c>
+      <c r="CI12">
+        <v>-0.0001733398703440877</v>
+      </c>
+      <c r="CJ12">
+        <v>-1.101098389793084E-06</v>
+      </c>
+      <c r="CK12">
+        <v>-0.00599098876921268</v>
+      </c>
+      <c r="CL12">
+        <v>-0.0008895961179376972</v>
+      </c>
+      <c r="CM12">
+        <v>-0.0001714547802201379</v>
+      </c>
+      <c r="CN12">
+        <v>-3.826712864624188E-06</v>
+      </c>
+      <c r="CO12">
+        <v>-0.0002785289953459669</v>
+      </c>
+      <c r="CP12">
+        <v>-9.977017557930129E-05</v>
+      </c>
+      <c r="CQ12">
+        <v>-2.103855832934659E-09</v>
+      </c>
+      <c r="CR12">
+        <v>-0.0001149417839375777</v>
+      </c>
+      <c r="CS12">
+        <v>-0.0001063923087018648</v>
+      </c>
+      <c r="CT12">
+        <v>-6.840513900650519E-05</v>
+      </c>
+      <c r="CU12">
+        <v>-2.367861380575093E-06</v>
+      </c>
+      <c r="CV12">
+        <v>-0.0008303236142377587</v>
+      </c>
+      <c r="CW12">
+        <v>-1.980473941110385E-05</v>
+      </c>
+      <c r="CX12">
+        <v>-0.0003270446488158221</v>
+      </c>
+      <c r="CY12">
+        <v>-0.01129320593084418</v>
+      </c>
+      <c r="CZ12">
+        <v>-0.004511670588210743</v>
+      </c>
+      <c r="DA12">
+        <v>-0.0001733389641522415</v>
+      </c>
+      <c r="DB12">
+        <v>-1.101098389793084E-06</v>
+      </c>
+      <c r="DC12">
+        <v>-0.0007515130076101416</v>
+      </c>
+      <c r="DD12">
+        <v>-0.0001934845451453056</v>
+      </c>
+      <c r="DE12">
+        <v>-0.0001133074848265907</v>
+      </c>
+      <c r="DF12">
+        <v>-3.826712864624188E-06</v>
+      </c>
+      <c r="DG12">
+        <v>-0.0002785289953459669</v>
+      </c>
+      <c r="DH12">
+        <v>-9.977017557930129E-05</v>
+      </c>
+      <c r="DI12">
+        <v>-2.103855832934659E-09</v>
+      </c>
+      <c r="DJ12">
+        <v>-0.0001149417839375777</v>
+      </c>
+      <c r="DK12">
+        <v>-0.0001063923087018648</v>
+      </c>
+      <c r="DL12">
+        <v>-6.210326375521939E-05</v>
+      </c>
+      <c r="DM12">
+        <v>-2.367664012913562E-06</v>
+      </c>
+      <c r="DN12">
+        <v>-0.0008303236142377587</v>
+      </c>
+      <c r="DO12">
+        <v>-1.980473941110385E-05</v>
+      </c>
+      <c r="DP12">
         <v>-0.004515747049010951</v>
       </c>
-      <c r="BO12">
+      <c r="DQ12">
         <v>-0.00315447096974555</v>
       </c>
-      <c r="BP12">
+      <c r="DR12">
         <v>-7.208915151740853E-06</v>
       </c>
-      <c r="BQ12">
+      <c r="DS12">
         <v>-0.01082660578102564</v>
       </c>
-      <c r="BR12">
+      <c r="DT12">
         <v>-2.108204589064716E-09</v>
       </c>
-      <c r="BS12">
+      <c r="DU12">
         <v>-8.954129970080758E-05</v>
       </c>
-      <c r="BT12">
+      <c r="DV12">
         <v>-7.179249395868318E-06</v>
       </c>
-      <c r="BU12">
+      <c r="DW12">
         <v>-0.2687987176873554</v>
       </c>
-      <c r="BV12">
+      <c r="DX12">
         <v>-3.387592784080466E-05</v>
       </c>
     </row>
-    <row r="13" spans="1:74">
+    <row r="13" spans="1:128">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C13">
         <v>0.0008116650470928445</v>
@@ -2954,39 +4772,201 @@
         <v>0.04464628927596968</v>
       </c>
       <c r="BN13">
+        <v>0.0168389473446827</v>
+      </c>
+      <c r="BO13">
+        <v>0.2348094522564988</v>
+      </c>
+      <c r="BP13">
+        <v>0.07205146744167908</v>
+      </c>
+      <c r="BQ13">
+        <v>0.006446162699534838</v>
+      </c>
+      <c r="BR13">
+        <v>6.237070170909272E-05</v>
+      </c>
+      <c r="BS13">
+        <v>3.373055305213053</v>
+      </c>
+      <c r="BT13">
+        <v>0.01499150524881549</v>
+      </c>
+      <c r="BU13">
+        <v>5.331614854226717</v>
+      </c>
+      <c r="BV13">
+        <v>6.754640493428138E-05</v>
+      </c>
+      <c r="BW13">
+        <v>0.1340983766674637</v>
+      </c>
+      <c r="BX13">
+        <v>-4.085579553857342E-05</v>
+      </c>
+      <c r="BY13">
+        <v>1.921140120583965E-08</v>
+      </c>
+      <c r="BZ13">
+        <v>0.0004419910003948514</v>
+      </c>
+      <c r="CA13">
+        <v>0.0009169802800336897</v>
+      </c>
+      <c r="CB13">
+        <v>0.0008872031054632986</v>
+      </c>
+      <c r="CC13">
+        <v>0.0003971933129873252</v>
+      </c>
+      <c r="CD13">
+        <v>0.01427819469452283</v>
+      </c>
+      <c r="CE13">
+        <v>0.002244325087477041</v>
+      </c>
+      <c r="CF13">
+        <v>0.0168389473446827</v>
+      </c>
+      <c r="CG13">
+        <v>0.243557586131211</v>
+      </c>
+      <c r="CH13">
+        <v>0.07205146744167908</v>
+      </c>
+      <c r="CI13">
+        <v>0.006410517879115097</v>
+      </c>
+      <c r="CJ13">
+        <v>6.237070170909272E-05</v>
+      </c>
+      <c r="CK13">
+        <v>0.06762944788573623</v>
+      </c>
+      <c r="CL13">
+        <v>0.01499150524881549</v>
+      </c>
+      <c r="CM13">
+        <v>0.005917043866140399</v>
+      </c>
+      <c r="CN13">
+        <v>6.754640493428138E-05</v>
+      </c>
+      <c r="CO13">
+        <v>0.1340983766674637</v>
+      </c>
+      <c r="CP13">
+        <v>-4.085579553857342E-05</v>
+      </c>
+      <c r="CQ13">
+        <v>1.921140120583965E-08</v>
+      </c>
+      <c r="CR13">
+        <v>0.0004419910003948514</v>
+      </c>
+      <c r="CS13">
+        <v>0.0009169802800336897</v>
+      </c>
+      <c r="CT13">
+        <v>0.0007853095393580742</v>
+      </c>
+      <c r="CU13">
+        <v>6.942454531975382E-05</v>
+      </c>
+      <c r="CV13">
+        <v>0.01427819469452283</v>
+      </c>
+      <c r="CW13">
+        <v>0.002244325087477041</v>
+      </c>
+      <c r="CX13">
+        <v>0.0168389473446827</v>
+      </c>
+      <c r="CY13">
+        <v>0.2651869596571065</v>
+      </c>
+      <c r="CZ13">
+        <v>0.07205146744167908</v>
+      </c>
+      <c r="DA13">
+        <v>0.006410460385204323</v>
+      </c>
+      <c r="DB13">
+        <v>6.237070170909272E-05</v>
+      </c>
+      <c r="DC13">
+        <v>0.01175397396603896</v>
+      </c>
+      <c r="DD13">
+        <v>0.007579569894613586</v>
+      </c>
+      <c r="DE13">
+        <v>0.00398439782760889</v>
+      </c>
+      <c r="DF13">
+        <v>6.754640493428138E-05</v>
+      </c>
+      <c r="DG13">
+        <v>0.1340983766674637</v>
+      </c>
+      <c r="DH13">
+        <v>-4.085579553857342E-05</v>
+      </c>
+      <c r="DI13">
+        <v>1.921140120583965E-08</v>
+      </c>
+      <c r="DJ13">
+        <v>0.0004419910003948514</v>
+      </c>
+      <c r="DK13">
+        <v>0.0009169802800336897</v>
+      </c>
+      <c r="DL13">
+        <v>0.0007344155032979094</v>
+      </c>
+      <c r="DM13">
+        <v>6.938829406923342E-05</v>
+      </c>
+      <c r="DN13">
+        <v>0.01427819469452283</v>
+      </c>
+      <c r="DO13">
+        <v>0.002244325087477041</v>
+      </c>
+      <c r="DP13">
         <v>0.04791341483706982</v>
       </c>
-      <c r="BO13">
+      <c r="DQ13">
         <v>0.1296891069755552</v>
       </c>
-      <c r="BP13">
+      <c r="DR13">
         <v>8.680258154695731E-05</v>
       </c>
-      <c r="BQ13">
+      <c r="DS13">
         <v>0.2437822862705943</v>
       </c>
-      <c r="BR13">
+      <c r="DT13">
         <v>1.985407474515192E-08</v>
       </c>
-      <c r="BS13">
+      <c r="DU13">
         <v>0.0006697063388449958</v>
       </c>
-      <c r="BT13">
+      <c r="DV13">
         <v>0.0003755314932486786</v>
       </c>
-      <c r="BU13">
+      <c r="DW13">
         <v>3.611478365970733</v>
       </c>
-      <c r="BV13">
+      <c r="DX13">
         <v>0.0002598748762516334</v>
       </c>
     </row>
-    <row r="14" spans="1:74">
+    <row r="14" spans="1:128">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C14">
         <v>0.0003030520355727356</v>
@@ -3178,39 +5158,201 @@
         <v>0.02721441936678227</v>
       </c>
       <c r="BN14">
+        <v>0.01697906681585396</v>
+      </c>
+      <c r="BO14">
+        <v>0.2040159530740195</v>
+      </c>
+      <c r="BP14">
+        <v>0.07597554189579732</v>
+      </c>
+      <c r="BQ14">
+        <v>0.003251148992606675</v>
+      </c>
+      <c r="BR14">
+        <v>2.941779533403164E-05</v>
+      </c>
+      <c r="BS14">
+        <v>1.67546724551404</v>
+      </c>
+      <c r="BT14">
+        <v>0.01024555706565074</v>
+      </c>
+      <c r="BU14">
+        <v>2.053147905255623</v>
+      </c>
+      <c r="BV14">
+        <v>4.253896406500993E-05</v>
+      </c>
+      <c r="BW14">
+        <v>0.01313603249720254</v>
+      </c>
+      <c r="BX14">
+        <v>-2.763593244586754E-05</v>
+      </c>
+      <c r="BY14">
+        <v>2.1685908278319E-08</v>
+      </c>
+      <c r="BZ14">
+        <v>0.0003391563129250328</v>
+      </c>
+      <c r="CA14">
+        <v>0.0007811674579990438</v>
+      </c>
+      <c r="CB14">
+        <v>0.0007768019083263663</v>
+      </c>
+      <c r="CC14">
+        <v>0.0003165288121127248</v>
+      </c>
+      <c r="CD14">
+        <v>0.01099176096105882</v>
+      </c>
+      <c r="CE14">
+        <v>0.0006395377123426806</v>
+      </c>
+      <c r="CF14">
+        <v>0.01697906681585396</v>
+      </c>
+      <c r="CG14">
+        <v>0.211254102549179</v>
+      </c>
+      <c r="CH14">
+        <v>0.07597554189579732</v>
+      </c>
+      <c r="CI14">
+        <v>0.003218152345926612</v>
+      </c>
+      <c r="CJ14">
+        <v>2.941779533403164E-05</v>
+      </c>
+      <c r="CK14">
+        <v>0.04016442110550985</v>
+      </c>
+      <c r="CL14">
+        <v>0.01024555706565074</v>
+      </c>
+      <c r="CM14">
+        <v>0.002934188254486859</v>
+      </c>
+      <c r="CN14">
+        <v>4.253896406500993E-05</v>
+      </c>
+      <c r="CO14">
+        <v>0.01313603249720254</v>
+      </c>
+      <c r="CP14">
+        <v>-2.763593244586754E-05</v>
+      </c>
+      <c r="CQ14">
+        <v>2.1685908278319E-08</v>
+      </c>
+      <c r="CR14">
+        <v>0.0003391563129250328</v>
+      </c>
+      <c r="CS14">
+        <v>0.0007811674579990438</v>
+      </c>
+      <c r="CT14">
+        <v>0.0006870970412632833</v>
+      </c>
+      <c r="CU14">
+        <v>3.511196859466081E-05</v>
+      </c>
+      <c r="CV14">
+        <v>0.01099176096105882</v>
+      </c>
+      <c r="CW14">
+        <v>0.0006395377123426806</v>
+      </c>
+      <c r="CX14">
+        <v>0.01697906681585396</v>
+      </c>
+      <c r="CY14">
+        <v>0.2292521830952508</v>
+      </c>
+      <c r="CZ14">
+        <v>0.07597554189579732</v>
+      </c>
+      <c r="DA14">
+        <v>0.003218029782599338</v>
+      </c>
+      <c r="DB14">
+        <v>2.941779533403164E-05</v>
+      </c>
+      <c r="DC14">
+        <v>0.008311375832313206</v>
+      </c>
+      <c r="DD14">
+        <v>0.004049620955294327</v>
+      </c>
+      <c r="DE14">
+        <v>0.001679424509229539</v>
+      </c>
+      <c r="DF14">
+        <v>4.253896406500993E-05</v>
+      </c>
+      <c r="DG14">
+        <v>0.01313603249720254</v>
+      </c>
+      <c r="DH14">
+        <v>-2.763593244586754E-05</v>
+      </c>
+      <c r="DI14">
+        <v>2.1685908278319E-08</v>
+      </c>
+      <c r="DJ14">
+        <v>0.0003391563129250328</v>
+      </c>
+      <c r="DK14">
+        <v>0.0007811674579990438</v>
+      </c>
+      <c r="DL14">
+        <v>0.0006437050991167255</v>
+      </c>
+      <c r="DM14">
+        <v>3.510472173865995E-05</v>
+      </c>
+      <c r="DN14">
+        <v>0.01099176096105882</v>
+      </c>
+      <c r="DO14">
+        <v>0.0006395377123426806</v>
+      </c>
+      <c r="DP14">
         <v>0.04218500218128832</v>
       </c>
-      <c r="BO14">
+      <c r="DQ14">
         <v>0.07238628474775788</v>
       </c>
-      <c r="BP14">
+      <c r="DR14">
         <v>5.773746094748009E-05</v>
       </c>
-      <c r="BQ14">
+      <c r="DS14">
         <v>0.2111963983851909</v>
       </c>
-      <c r="BR14">
+      <c r="DT14">
         <v>2.18857357958245E-08</v>
       </c>
-      <c r="BS14">
+      <c r="DU14">
         <v>0.000623319722841974</v>
       </c>
-      <c r="BT14">
+      <c r="DV14">
         <v>0.0001891404200420736</v>
       </c>
-      <c r="BU14">
+      <c r="DW14">
         <v>3.309303120579779</v>
       </c>
-      <c r="BV14">
+      <c r="DX14">
         <v>0.0001945008510398676</v>
       </c>
     </row>
-    <row r="15" spans="1:74">
+    <row r="15" spans="1:128">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C15">
         <v>0.003467084616428644</v>
@@ -3402,39 +5544,204 @@
         <v>0.1238154606128195</v>
       </c>
       <c r="BN15">
+        <v>0.0314988029243552</v>
+      </c>
+      <c r="BO15">
+        <v>0.5553389310745553</v>
+      </c>
+      <c r="BP15">
+        <v>0.1554145592714853</v>
+      </c>
+      <c r="BQ15">
+        <v>0.02655420357129178</v>
+      </c>
+      <c r="BR15">
+        <v>0.0002488511430205342</v>
+      </c>
+      <c r="BS15">
+        <v>13.18602289695679</v>
+      </c>
+      <c r="BT15">
+        <v>0.04670204504936146</v>
+      </c>
+      <c r="BU15">
+        <v>23.67844057981528</v>
+      </c>
+      <c r="BV15">
+        <v>0.0002054034410355788</v>
+      </c>
+      <c r="BW15">
+        <v>0.4444255056402289</v>
+      </c>
+      <c r="BX15">
+        <v>1.865919207605458E-06</v>
+      </c>
+      <c r="BY15">
+        <v>3.621534406050502E-08</v>
+      </c>
+      <c r="BZ15">
+        <v>0.001381535289399253</v>
+      </c>
+      <c r="CA15">
+        <v>0.002329863568001287</v>
+      </c>
+      <c r="CB15">
+        <v>0.002235144332670227</v>
+      </c>
+      <c r="CC15">
+        <v>0.001214818331517639</v>
+      </c>
+      <c r="CD15">
+        <v>0.04483701949788843</v>
+      </c>
+      <c r="CE15">
+        <v>0.008631071134479874</v>
+      </c>
+      <c r="CF15">
+        <v>0.0314988029243552</v>
+      </c>
+      <c r="CG15">
+        <v>0.5774063070122285</v>
+      </c>
+      <c r="CH15">
+        <v>0.1554145592714853</v>
+      </c>
+      <c r="CI15">
+        <v>0.02646331348788647</v>
+      </c>
+      <c r="CJ15">
+        <v>0.0002488511430205342</v>
+      </c>
+      <c r="CK15">
+        <v>0.2506815087422659</v>
+      </c>
+      <c r="CL15">
+        <v>0.04670204504936146</v>
+      </c>
+      <c r="CM15">
+        <v>0.02463743650433387</v>
+      </c>
+      <c r="CN15">
+        <v>0.0002054034410355788</v>
+      </c>
+      <c r="CO15">
+        <v>0.4444255056402289</v>
+      </c>
+      <c r="CP15">
+        <v>1.865919207605458E-06</v>
+      </c>
+      <c r="CQ15">
+        <v>3.621534406050502E-08</v>
+      </c>
+      <c r="CR15">
+        <v>0.001381535289399253</v>
+      </c>
+      <c r="CS15">
+        <v>0.002329863568001287</v>
+      </c>
+      <c r="CT15">
+        <v>0.002006332817447511</v>
+      </c>
+      <c r="CU15">
+        <v>0.0002315381533710673</v>
+      </c>
+      <c r="CV15">
+        <v>0.04483701949788843</v>
+      </c>
+      <c r="CW15">
+        <v>0.008631071134479874</v>
+      </c>
+      <c r="CX15">
+        <v>0.0314988029243552</v>
+      </c>
+      <c r="CY15">
+        <v>0.6325824031908578</v>
+      </c>
+      <c r="CZ15">
+        <v>0.1554145592714853</v>
+      </c>
+      <c r="DA15">
+        <v>0.02646323236315593</v>
+      </c>
+      <c r="DB15">
+        <v>0.0002488511430205342</v>
+      </c>
+      <c r="DC15">
+        <v>0.03629858145800273</v>
+      </c>
+      <c r="DD15">
+        <v>0.02647078317277649</v>
+      </c>
+      <c r="DE15">
+        <v>0.01764383089232802</v>
+      </c>
+      <c r="DF15">
+        <v>0.0002054034410355788</v>
+      </c>
+      <c r="DG15">
+        <v>0.4444255056402289</v>
+      </c>
+      <c r="DH15">
+        <v>1.865919207605458E-06</v>
+      </c>
+      <c r="DI15">
+        <v>3.621534406050502E-08</v>
+      </c>
+      <c r="DJ15">
+        <v>0.001381535289399253</v>
+      </c>
+      <c r="DK15">
+        <v>0.002329863568001287</v>
+      </c>
+      <c r="DL15">
+        <v>0.001891200468116588</v>
+      </c>
+      <c r="DM15">
+        <v>0.0002315101096181764</v>
+      </c>
+      <c r="DN15">
+        <v>0.04483701949788843</v>
+      </c>
+      <c r="DO15">
+        <v>0.008631071134479874</v>
+      </c>
+      <c r="DP15">
         <v>0.1197011458648232</v>
       </c>
-      <c r="BO15">
+      <c r="DQ15">
         <v>0.5026693746178221</v>
       </c>
-      <c r="BP15">
+      <c r="DR15">
         <v>0.0003009713527151938</v>
       </c>
-      <c r="BQ15">
+      <c r="DS15">
         <v>0.5789625500590913</v>
       </c>
-      <c r="BR15">
+      <c r="DT15">
         <v>3.958524011484141E-08</v>
       </c>
-      <c r="BS15">
+      <c r="DU15">
         <v>0.001502224780763798</v>
       </c>
-      <c r="BT15">
+      <c r="DV15">
         <v>0.001538875651449092</v>
       </c>
-      <c r="BU15">
+      <c r="DW15">
         <v>10.11615219276999</v>
       </c>
-      <c r="BV15">
+      <c r="DX15">
         <v>0.0007970328255974815</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="18">
     <mergeCell ref="C1:W1"/>
     <mergeCell ref="X1:AR1"/>
     <mergeCell ref="AS1:BM1"/>
-    <mergeCell ref="BN1:BV1"/>
+    <mergeCell ref="BN1:CE1"/>
+    <mergeCell ref="CF1:CW1"/>
+    <mergeCell ref="CX1:DO1"/>
+    <mergeCell ref="DP1:DX1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="M2:S2"/>
     <mergeCell ref="T2:V2"/>
@@ -3444,8 +5751,8 @@
     <mergeCell ref="AS2:BB2"/>
     <mergeCell ref="BC2:BI2"/>
     <mergeCell ref="BJ2:BL2"/>
-    <mergeCell ref="BN2:BS2"/>
-    <mergeCell ref="BT2:BV2"/>
+    <mergeCell ref="DP2:DU2"/>
+    <mergeCell ref="DV2:DX2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>